<commit_message>
Revert "[feat] 아이템Data에 _exp value추가"
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Item/RawData/ItemDBSheet.xlsx
+++ b/Assets/Scripts/Item/RawData/ItemDBSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMS\Desktop\Mementomori\Assets\Scripts\Item\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B85BAE-A99C-4851-AB2D-35A0BD830373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF159601-0BF7-46ED-A600-C2C18DBCFCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EEB29282-1E6A-43A2-9D10-8454725A0340}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="159">
   <si>
     <t>_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -656,6 +656,10 @@
   </si>
   <si>
     <t>Sprite/Item/Exp/exp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_exp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1023,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9413D641-5D00-473F-AAE5-77EBB53F717C}">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1041,7 +1045,7 @@
     <col min="10" max="10" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1078,8 +1082,11 @@
       <c r="L1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10001001</v>
       </c>
@@ -1109,7 +1116,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10001002</v>
       </c>
@@ -1139,7 +1146,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10001003</v>
       </c>
@@ -1169,7 +1176,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10001004</v>
       </c>
@@ -1199,7 +1206,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10001005</v>
       </c>
@@ -1229,7 +1236,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10001006</v>
       </c>
@@ -1259,7 +1266,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10001007</v>
       </c>
@@ -1289,7 +1296,7 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10001008</v>
       </c>
@@ -1319,7 +1326,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10001009</v>
       </c>
@@ -1349,7 +1356,7 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10001010</v>
       </c>
@@ -1379,7 +1386,7 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10001011</v>
       </c>
@@ -1409,7 +1416,7 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10001012</v>
       </c>
@@ -1439,7 +1446,7 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>20001001</v>
       </c>
@@ -1467,7 +1474,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>20001002</v>
       </c>
@@ -1495,7 +1502,7 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>20001003</v>
       </c>
@@ -2441,7 +2448,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>40001024</v>
       </c>
@@ -2471,7 +2478,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>50001000</v>
       </c>
@@ -2483,6 +2490,9 @@
       </c>
       <c r="F50" t="s">
         <v>157</v>
+      </c>
+      <c r="M50">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>